<commit_message>
El día de hoy corregí las cagaderas, ya está listo para los análisis conductuales
</commit_message>
<xml_diff>
--- a/Demograficos.xlsx
+++ b/Demograficos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f3ba38939858e1d/Documentos/WM^0Att Edad adulta/Bases de datos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\elissa\Analisis\Analisis-R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="204" documentId="11_DB0F378A269C8C3F69A79A300FD754EA951298C4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F28F2017-4FCF-45D0-8807-9271B1A7A3A9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97588061-7EA8-4918-A7B5-83611E2CAF4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="20" sheetId="1" r:id="rId1"/>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1722" uniqueCount="808">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1720" uniqueCount="808">
   <si>
     <t>ID</t>
   </si>
@@ -12340,7 +12340,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AG1001"/>
   <sheetViews>
-    <sheetView topLeftCell="L16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="AD30" sqref="AD30:AE30"/>
     </sheetView>
   </sheetViews>
@@ -29203,7 +29203,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AG1001"/>
   <sheetViews>
-    <sheetView topLeftCell="J31" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="AD61" sqref="AD61:AE61"/>
     </sheetView>
   </sheetViews>
@@ -37834,8 +37834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AG1006"/>
   <sheetViews>
-    <sheetView topLeftCell="L25" workbookViewId="0">
-      <selection activeCell="AD52" sqref="AD52:AE52"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="R47" sqref="R47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -45589,11 +45589,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:AG960"/>
+  <dimension ref="A1:AG959"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A194" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I182" sqref="I182"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K214" sqref="K214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -66115,110 +66115,110 @@
         <v>5534119535</v>
       </c>
     </row>
-    <row r="204" spans="1:33" s="165" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A204" s="203" t="s">
-        <v>698</v>
-      </c>
-      <c r="B204" s="203">
+    <row r="204" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A204" s="208" t="s">
+        <v>700</v>
+      </c>
+      <c r="B204" s="171">
         <v>60</v>
       </c>
-      <c r="C204" s="203">
-        <v>1</v>
-      </c>
-      <c r="D204" s="213">
-        <v>65</v>
-      </c>
-      <c r="E204" s="213">
-        <v>29</v>
-      </c>
-      <c r="F204" s="213">
-        <v>20</v>
-      </c>
-      <c r="G204" s="213">
-        <v>0</v>
-      </c>
-      <c r="H204" s="213">
-        <v>20</v>
-      </c>
-      <c r="I204" s="213">
-        <v>96</v>
-      </c>
-      <c r="J204" s="213">
+      <c r="C204" s="171">
+        <v>2</v>
+      </c>
+      <c r="D204" s="171">
+        <v>66</v>
+      </c>
+      <c r="E204" s="183">
+        <v>26</v>
+      </c>
+      <c r="F204" s="172">
+        <v>25</v>
+      </c>
+      <c r="G204" s="172">
+        <v>1.5</v>
+      </c>
+      <c r="H204" s="172">
+        <v>26.5</v>
+      </c>
+      <c r="I204" s="172">
         <v>151</v>
       </c>
-      <c r="K204" s="213">
-        <v>195</v>
-      </c>
-      <c r="L204" s="213">
-        <v>163</v>
-      </c>
-      <c r="M204" s="177">
-        <v>0</v>
-      </c>
-      <c r="N204" s="177">
-        <v>0</v>
-      </c>
-      <c r="O204" s="177">
-        <v>0</v>
-      </c>
-      <c r="P204" s="214">
-        <v>44593</v>
-      </c>
-      <c r="Q204" s="177">
-        <v>4</v>
-      </c>
-      <c r="R204" s="177">
-        <v>89.47</v>
-      </c>
-      <c r="S204" s="177">
-        <v>39</v>
-      </c>
-      <c r="T204" s="177">
-        <v>2</v>
-      </c>
-      <c r="U204" s="177">
+      <c r="J204" s="172">
+        <v>169</v>
+      </c>
+      <c r="K204" s="172">
+        <v>107</v>
+      </c>
+      <c r="L204" s="172">
+        <v>156</v>
+      </c>
+      <c r="M204" s="168">
+        <v>0</v>
+      </c>
+      <c r="N204" s="169">
+        <v>0</v>
+      </c>
+      <c r="O204" s="169">
+        <v>0</v>
+      </c>
+      <c r="P204" s="177">
+        <v>0</v>
+      </c>
+      <c r="Q204" s="169">
+        <v>0</v>
+      </c>
+      <c r="R204" s="169">
+        <v>100</v>
+      </c>
+      <c r="S204" s="169">
+        <v>42</v>
+      </c>
+      <c r="T204" s="169">
+        <v>2</v>
+      </c>
+      <c r="U204" s="169">
+        <v>41</v>
+      </c>
+      <c r="V204" s="169">
+        <v>2</v>
+      </c>
+      <c r="W204" s="169">
         <v>48</v>
       </c>
-      <c r="V204" s="177">
-        <v>3</v>
-      </c>
-      <c r="W204" s="177">
-        <v>45</v>
-      </c>
-      <c r="X204" s="177">
-        <v>2</v>
+      <c r="X204" s="169">
+        <v>3</v>
       </c>
       <c r="Y204" s="177">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="Z204" s="177">
-        <v>3</v>
-      </c>
-      <c r="AA204" s="177">
-        <v>105</v>
-      </c>
-      <c r="AB204" s="177">
-        <v>124</v>
-      </c>
-      <c r="AC204" s="177">
-        <v>117</v>
-      </c>
-      <c r="AD204" s="177">
+        <v>2</v>
+      </c>
+      <c r="AA204" s="212">
+        <v>109.62962962962963</v>
+      </c>
+      <c r="AB204" s="212">
+        <v>110.62962962962963</v>
+      </c>
+      <c r="AC204" s="212">
+        <v>112</v>
+      </c>
+      <c r="AD204" s="185">
         <v>8</v>
       </c>
-      <c r="AE204" s="177">
+      <c r="AE204" s="185">
         <v>8</v>
       </c>
-      <c r="AF204" s="177" t="s">
-        <v>699</v>
-      </c>
-      <c r="AG204" s="170">
-        <v>5518381087</v>
+      <c r="AF204" s="169" t="s">
+        <v>701</v>
+      </c>
+      <c r="AG204" s="170" t="s">
+        <v>702</v>
       </c>
     </row>
     <row r="205" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A205" s="208" t="s">
-        <v>700</v>
+      <c r="A205" s="171" t="s">
+        <v>703</v>
       </c>
       <c r="B205" s="171">
         <v>60</v>
@@ -66226,32 +66226,32 @@
       <c r="C205" s="171">
         <v>2</v>
       </c>
-      <c r="D205" s="171">
-        <v>66</v>
-      </c>
-      <c r="E205" s="183">
-        <v>26</v>
+      <c r="D205" s="172">
+        <v>64</v>
+      </c>
+      <c r="E205" s="172">
+        <v>27</v>
       </c>
       <c r="F205" s="172">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G205" s="172">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="H205" s="172">
-        <v>26.5</v>
+        <v>20</v>
       </c>
       <c r="I205" s="172">
-        <v>151</v>
+        <v>129</v>
       </c>
       <c r="J205" s="172">
-        <v>169</v>
+        <v>119</v>
       </c>
       <c r="K205" s="172">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="L205" s="172">
-        <v>156</v>
+        <v>118</v>
       </c>
       <c r="M205" s="168">
         <v>0</v>
@@ -66260,7 +66260,7 @@
         <v>0</v>
       </c>
       <c r="O205" s="169">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P205" s="177">
         <v>0</v>
@@ -66272,7 +66272,7 @@
         <v>100</v>
       </c>
       <c r="S205" s="169">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T205" s="169">
         <v>2</v>
@@ -66284,42 +66284,42 @@
         <v>2</v>
       </c>
       <c r="W205" s="169">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="X205" s="169">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Y205" s="177">
-        <v>40</v>
-      </c>
-      <c r="Z205" s="177">
-        <v>2</v>
-      </c>
-      <c r="AA205" s="212">
-        <v>109.62962962962963</v>
-      </c>
-      <c r="AB205" s="212">
-        <v>110.62962962962963</v>
-      </c>
-      <c r="AC205" s="212">
-        <v>112</v>
+        <v>43</v>
+      </c>
+      <c r="Z205" s="169">
+        <v>3</v>
+      </c>
+      <c r="AA205" s="168">
+        <v>103</v>
+      </c>
+      <c r="AB205" s="168">
+        <v>105</v>
+      </c>
+      <c r="AC205" s="168">
+        <v>105</v>
       </c>
       <c r="AD205" s="185">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AE205" s="185">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AF205" s="169" t="s">
-        <v>701</v>
+        <v>704</v>
       </c>
       <c r="AG205" s="170" t="s">
-        <v>702</v>
+        <v>705</v>
       </c>
     </row>
     <row r="206" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="171" t="s">
-        <v>703</v>
+        <v>707</v>
       </c>
       <c r="B206" s="171">
         <v>60</v>
@@ -66328,32 +66328,32 @@
         <v>2</v>
       </c>
       <c r="D206" s="172">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="E206" s="172">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F206" s="172">
-        <v>20</v>
+        <v>13.5</v>
       </c>
       <c r="G206" s="172">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H206" s="172">
-        <v>20</v>
+        <v>16.5</v>
       </c>
       <c r="I206" s="172">
+        <v>121</v>
+      </c>
+      <c r="J206" s="172">
+        <v>114</v>
+      </c>
+      <c r="K206" s="172">
+        <v>132</v>
+      </c>
+      <c r="L206" s="172">
         <v>129</v>
       </c>
-      <c r="J206" s="172">
-        <v>119</v>
-      </c>
-      <c r="K206" s="172">
-        <v>93</v>
-      </c>
-      <c r="L206" s="172">
-        <v>118</v>
-      </c>
       <c r="M206" s="168">
         <v>0</v>
       </c>
@@ -66361,7 +66361,7 @@
         <v>0</v>
       </c>
       <c r="O206" s="169">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P206" s="177">
         <v>0</v>
@@ -66370,57 +66370,57 @@
         <v>0</v>
       </c>
       <c r="R206" s="169">
-        <v>100</v>
+        <v>65.22</v>
       </c>
       <c r="S206" s="169">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="T206" s="169">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U206" s="169">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="V206" s="169">
         <v>2</v>
       </c>
-      <c r="W206" s="169">
-        <v>43</v>
-      </c>
-      <c r="X206" s="169">
+      <c r="W206" s="177">
+        <v>37</v>
+      </c>
+      <c r="X206" s="177">
         <v>2</v>
       </c>
       <c r="Y206" s="177">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="Z206" s="169">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AA206" s="168">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="AB206" s="168">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="AC206" s="168">
-        <v>105</v>
-      </c>
-      <c r="AD206" s="185">
-        <v>7</v>
-      </c>
-      <c r="AE206" s="185">
-        <v>7</v>
+        <v>106</v>
+      </c>
+      <c r="AD206" s="173">
+        <v>6.9</v>
+      </c>
+      <c r="AE206" s="173">
+        <v>6.6</v>
       </c>
       <c r="AF206" s="169" t="s">
-        <v>704</v>
+        <v>708</v>
       </c>
       <c r="AG206" s="170" t="s">
-        <v>705</v>
+        <v>709</v>
       </c>
     </row>
     <row r="207" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="171" t="s">
-        <v>707</v>
+        <v>710</v>
       </c>
       <c r="B207" s="171">
         <v>60</v>
@@ -66429,31 +66429,31 @@
         <v>2</v>
       </c>
       <c r="D207" s="172">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E207" s="172">
         <v>26</v>
       </c>
       <c r="F207" s="172">
-        <v>13.5</v>
+        <v>17</v>
       </c>
       <c r="G207" s="172">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="H207" s="172">
-        <v>16.5</v>
+        <v>17.5</v>
       </c>
       <c r="I207" s="172">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J207" s="172">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="K207" s="172">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L207" s="172">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="M207" s="168">
         <v>0</v>
@@ -66461,8 +66461,8 @@
       <c r="N207" s="169">
         <v>0</v>
       </c>
-      <c r="O207" s="169">
-        <v>0</v>
+      <c r="O207" s="177">
+        <v>1</v>
       </c>
       <c r="P207" s="177">
         <v>0</v>
@@ -66471,40 +66471,40 @@
         <v>0</v>
       </c>
       <c r="R207" s="169">
-        <v>65.22</v>
+        <v>100</v>
       </c>
       <c r="S207" s="169">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="T207" s="169">
         <v>3</v>
       </c>
       <c r="U207" s="169">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="V207" s="169">
-        <v>2</v>
-      </c>
-      <c r="W207" s="177">
-        <v>37</v>
-      </c>
-      <c r="X207" s="177">
-        <v>2</v>
-      </c>
-      <c r="Y207" s="177">
-        <v>39</v>
+        <v>3</v>
+      </c>
+      <c r="W207" s="169">
+        <v>52</v>
+      </c>
+      <c r="X207" s="169">
+        <v>3</v>
+      </c>
+      <c r="Y207" s="169">
+        <v>48</v>
       </c>
       <c r="Z207" s="169">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA207" s="168">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="AB207" s="168">
-        <v>96</v>
+        <v>131</v>
       </c>
       <c r="AC207" s="168">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="AD207" s="173">
         <v>6.9</v>
@@ -66513,15 +66513,15 @@
         <v>6.6</v>
       </c>
       <c r="AF207" s="169" t="s">
-        <v>708</v>
+        <v>711</v>
       </c>
       <c r="AG207" s="170" t="s">
-        <v>709</v>
+        <v>712</v>
       </c>
     </row>
     <row r="208" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="171" t="s">
-        <v>710</v>
+        <v>714</v>
       </c>
       <c r="B208" s="171">
         <v>60</v>
@@ -66529,32 +66529,32 @@
       <c r="C208" s="171">
         <v>2</v>
       </c>
-      <c r="D208" s="172">
-        <v>60</v>
-      </c>
-      <c r="E208" s="172">
-        <v>26</v>
+      <c r="D208" s="171">
+        <v>66</v>
+      </c>
+      <c r="E208" s="183">
+        <v>27</v>
       </c>
       <c r="F208" s="172">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G208" s="172">
-        <v>0.5</v>
+        <v>6</v>
       </c>
       <c r="H208" s="172">
-        <v>17.5</v>
+        <v>18</v>
       </c>
       <c r="I208" s="172">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="J208" s="172">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K208" s="172">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="L208" s="172">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M208" s="168">
         <v>0</v>
@@ -66562,67 +66562,67 @@
       <c r="N208" s="169">
         <v>0</v>
       </c>
-      <c r="O208" s="177">
-        <v>1</v>
-      </c>
-      <c r="P208" s="177">
-        <v>0</v>
-      </c>
-      <c r="Q208" s="169">
-        <v>0</v>
+      <c r="O208" s="169">
+        <v>0</v>
+      </c>
+      <c r="P208" s="227">
+        <v>44018</v>
+      </c>
+      <c r="Q208" s="224" t="s">
+        <v>715</v>
       </c>
       <c r="R208" s="169">
         <v>100</v>
       </c>
       <c r="S208" s="169">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="T208" s="169">
         <v>3</v>
       </c>
       <c r="U208" s="169">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="V208" s="169">
         <v>3</v>
       </c>
       <c r="W208" s="169">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="X208" s="169">
-        <v>3</v>
-      </c>
-      <c r="Y208" s="169">
-        <v>48</v>
+        <v>2</v>
+      </c>
+      <c r="Y208" s="177">
+        <v>44</v>
       </c>
       <c r="Z208" s="169">
         <v>3</v>
       </c>
       <c r="AA208" s="168">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="AB208" s="168">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="AC208" s="168">
-        <v>122</v>
-      </c>
-      <c r="AD208" s="173">
-        <v>6.9</v>
-      </c>
-      <c r="AE208" s="173">
-        <v>6.6</v>
+        <v>119</v>
+      </c>
+      <c r="AD208" s="168">
+        <v>7</v>
+      </c>
+      <c r="AE208" s="168">
+        <v>7</v>
       </c>
       <c r="AF208" s="169" t="s">
-        <v>711</v>
+        <v>716</v>
       </c>
       <c r="AG208" s="170" t="s">
-        <v>712</v>
+        <v>717</v>
       </c>
     </row>
     <row r="209" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="171" t="s">
-        <v>714</v>
+        <v>718</v>
       </c>
       <c r="B209" s="171">
         <v>60</v>
@@ -66630,32 +66630,32 @@
       <c r="C209" s="171">
         <v>2</v>
       </c>
-      <c r="D209" s="171">
-        <v>66</v>
-      </c>
-      <c r="E209" s="183">
-        <v>27</v>
+      <c r="D209" s="172">
+        <v>64</v>
+      </c>
+      <c r="E209" s="172">
+        <v>28</v>
       </c>
       <c r="F209" s="172">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G209" s="172">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H209" s="172">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I209" s="172">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="J209" s="172">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="K209" s="172">
-        <v>124</v>
+        <v>93</v>
       </c>
       <c r="L209" s="172">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="M209" s="168">
         <v>0</v>
@@ -66666,64 +66666,64 @@
       <c r="O209" s="169">
         <v>0</v>
       </c>
-      <c r="P209" s="227">
-        <v>44018</v>
-      </c>
-      <c r="Q209" s="224" t="s">
-        <v>715</v>
+      <c r="P209" s="177">
+        <v>0</v>
+      </c>
+      <c r="Q209" s="169">
+        <v>0</v>
       </c>
       <c r="R209" s="169">
-        <v>100</v>
+        <v>90.91</v>
       </c>
       <c r="S209" s="169">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="T209" s="169">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U209" s="169">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="V209" s="169">
         <v>3</v>
       </c>
       <c r="W209" s="169">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="X209" s="169">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y209" s="177">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="Z209" s="169">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AA209" s="168">
         <v>111</v>
       </c>
       <c r="AB209" s="168">
+        <v>124</v>
+      </c>
+      <c r="AC209" s="168">
         <v>121</v>
-      </c>
-      <c r="AC209" s="168">
-        <v>119</v>
       </c>
       <c r="AD209" s="168">
         <v>7</v>
       </c>
       <c r="AE209" s="168">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AF209" s="169" t="s">
-        <v>716</v>
+        <v>719</v>
       </c>
       <c r="AG209" s="170" t="s">
-        <v>717</v>
+        <v>720</v>
       </c>
     </row>
     <row r="210" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="171" t="s">
-        <v>718</v>
+        <v>721</v>
       </c>
       <c r="B210" s="171">
         <v>60</v>
@@ -66732,37 +66732,37 @@
         <v>2</v>
       </c>
       <c r="D210" s="172">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E210" s="172">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F210" s="172">
+        <v>14</v>
+      </c>
+      <c r="G210" s="172">
+        <v>2</v>
+      </c>
+      <c r="H210" s="172">
         <v>16</v>
       </c>
-      <c r="G210" s="172">
-        <v>3</v>
-      </c>
-      <c r="H210" s="172">
-        <v>19</v>
-      </c>
       <c r="I210" s="172">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="J210" s="172">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="K210" s="172">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="L210" s="172">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="M210" s="168">
         <v>0</v>
       </c>
-      <c r="N210" s="169">
-        <v>0</v>
+      <c r="N210" s="177">
+        <v>1</v>
       </c>
       <c r="O210" s="169">
         <v>0</v>
@@ -66774,57 +66774,57 @@
         <v>0</v>
       </c>
       <c r="R210" s="169">
-        <v>90.91</v>
+        <v>91.3</v>
       </c>
       <c r="S210" s="169">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="T210" s="169">
         <v>2</v>
       </c>
       <c r="U210" s="169">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="V210" s="169">
         <v>3</v>
       </c>
       <c r="W210" s="169">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X210" s="169">
         <v>3</v>
       </c>
       <c r="Y210" s="177">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="Z210" s="169">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA210" s="168">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="AB210" s="168">
         <v>124</v>
       </c>
       <c r="AC210" s="168">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="AD210" s="168">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="AE210" s="168">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="AF210" s="169" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="AG210" s="170" t="s">
-        <v>720</v>
+        <v>723</v>
       </c>
     </row>
     <row r="211" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="171" t="s">
-        <v>721</v>
+        <v>724</v>
       </c>
       <c r="B211" s="171">
         <v>60</v>
@@ -66836,28 +66836,28 @@
         <v>63</v>
       </c>
       <c r="E211" s="172">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F211" s="172">
-        <v>14</v>
+        <v>16.5</v>
       </c>
       <c r="G211" s="172">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H211" s="172">
-        <v>16</v>
+        <v>17.5</v>
       </c>
       <c r="I211" s="172">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="J211" s="172">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="K211" s="172">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="L211" s="172">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="M211" s="168">
         <v>0</v>
@@ -66875,57 +66875,57 @@
         <v>0</v>
       </c>
       <c r="R211" s="169">
-        <v>91.3</v>
+        <v>72.73</v>
       </c>
       <c r="S211" s="169">
+        <v>43</v>
+      </c>
+      <c r="T211" s="169">
+        <v>2</v>
+      </c>
+      <c r="U211" s="169">
+        <v>40</v>
+      </c>
+      <c r="V211" s="169">
+        <v>2</v>
+      </c>
+      <c r="W211" s="169">
         <v>44</v>
       </c>
-      <c r="T211" s="169">
-        <v>2</v>
-      </c>
-      <c r="U211" s="169">
-        <v>45</v>
-      </c>
-      <c r="V211" s="169">
-        <v>3</v>
-      </c>
-      <c r="W211" s="169">
-        <v>50</v>
-      </c>
       <c r="X211" s="169">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Y211" s="177">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="Z211" s="169">
         <v>3</v>
       </c>
       <c r="AA211" s="168">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="AB211" s="168">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="AC211" s="168">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="AD211" s="168">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AE211" s="168">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AF211" s="169" t="s">
-        <v>722</v>
+        <v>725</v>
       </c>
       <c r="AG211" s="170" t="s">
-        <v>723</v>
+        <v>726</v>
       </c>
     </row>
     <row r="212" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="171" t="s">
-        <v>724</v>
+        <v>727</v>
       </c>
       <c r="B212" s="171">
         <v>60</v>
@@ -66934,31 +66934,31 @@
         <v>2</v>
       </c>
       <c r="D212" s="172">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E212" s="172">
         <v>27</v>
       </c>
       <c r="F212" s="172">
-        <v>16.5</v>
+        <v>16</v>
       </c>
       <c r="G212" s="172">
         <v>1</v>
       </c>
       <c r="H212" s="172">
-        <v>17.5</v>
+        <v>17</v>
       </c>
       <c r="I212" s="172">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J212" s="172">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="K212" s="172">
-        <v>98</v>
+        <v>127</v>
       </c>
       <c r="L212" s="172">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="M212" s="168">
         <v>0</v>
@@ -66969,64 +66969,64 @@
       <c r="O212" s="169">
         <v>0</v>
       </c>
-      <c r="P212" s="177">
-        <v>0</v>
+      <c r="P212" s="227">
+        <v>44560</v>
       </c>
       <c r="Q212" s="169">
         <v>0</v>
       </c>
       <c r="R212" s="169">
-        <v>72.73</v>
+        <v>100</v>
       </c>
       <c r="S212" s="169">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="T212" s="169">
         <v>2</v>
       </c>
       <c r="U212" s="169">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="V212" s="169">
         <v>2</v>
       </c>
       <c r="W212" s="169">
+        <v>47</v>
+      </c>
+      <c r="X212" s="169">
+        <v>3</v>
+      </c>
+      <c r="Y212" s="177">
         <v>44</v>
       </c>
-      <c r="X212" s="169">
-        <v>2</v>
-      </c>
-      <c r="Y212" s="177">
-        <v>46</v>
-      </c>
       <c r="Z212" s="169">
         <v>3</v>
       </c>
       <c r="AA212" s="168">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="AB212" s="168">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AC212" s="168">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="AD212" s="168">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="AE212" s="168">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AF212" s="169" t="s">
-        <v>725</v>
+        <v>728</v>
       </c>
       <c r="AG212" s="170" t="s">
-        <v>726</v>
+        <v>729</v>
       </c>
     </row>
     <row r="213" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="171" t="s">
-        <v>727</v>
+        <v>730</v>
       </c>
       <c r="B213" s="171">
         <v>60</v>
@@ -67035,67 +67035,67 @@
         <v>2</v>
       </c>
       <c r="D213" s="172">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E213" s="172">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F213" s="172">
+        <v>12</v>
+      </c>
+      <c r="G213" s="172">
+        <v>4</v>
+      </c>
+      <c r="H213" s="172">
         <v>16</v>
       </c>
-      <c r="G213" s="172">
-        <v>1</v>
-      </c>
-      <c r="H213" s="172">
-        <v>17</v>
-      </c>
       <c r="I213" s="172">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="J213" s="172">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="K213" s="172">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L213" s="172">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="M213" s="168">
         <v>0</v>
       </c>
-      <c r="N213" s="177">
-        <v>1</v>
+      <c r="N213" s="169">
+        <v>0</v>
       </c>
       <c r="O213" s="169">
         <v>0</v>
       </c>
-      <c r="P213" s="227">
-        <v>44560</v>
+      <c r="P213" s="177">
+        <v>0</v>
       </c>
       <c r="Q213" s="169">
         <v>0</v>
       </c>
       <c r="R213" s="169">
-        <v>100</v>
+        <v>83.33</v>
       </c>
       <c r="S213" s="169">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="T213" s="169">
         <v>2</v>
       </c>
       <c r="U213" s="169">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="V213" s="169">
         <v>2</v>
       </c>
       <c r="W213" s="169">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="X213" s="169">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Y213" s="177">
         <v>44</v>
@@ -67104,30 +67104,30 @@
         <v>3</v>
       </c>
       <c r="AA213" s="168">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AB213" s="168">
-        <v>93</v>
+        <v>118</v>
       </c>
       <c r="AC213" s="168">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="AD213" s="168">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AE213" s="168">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AF213" s="169" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="AG213" s="170" t="s">
-        <v>729</v>
+        <v>732</v>
       </c>
     </row>
     <row r="214" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="171" t="s">
-        <v>730</v>
+        <v>733</v>
       </c>
       <c r="B214" s="171">
         <v>60</v>
@@ -67136,28 +67136,28 @@
         <v>2</v>
       </c>
       <c r="D214" s="172">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="E214" s="172">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F214" s="172">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G214" s="172">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H214" s="172">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I214" s="172">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="J214" s="172">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="K214" s="172">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="L214" s="172">
         <v>111</v>
@@ -67171,14 +67171,14 @@
       <c r="O214" s="169">
         <v>0</v>
       </c>
-      <c r="P214" s="177">
-        <v>0</v>
+      <c r="P214" s="227">
+        <v>44746</v>
       </c>
       <c r="Q214" s="169">
         <v>0</v>
       </c>
       <c r="R214" s="169">
-        <v>83.33</v>
+        <v>91.67</v>
       </c>
       <c r="S214" s="169">
         <v>42</v>
@@ -67187,13 +67187,13 @@
         <v>2</v>
       </c>
       <c r="U214" s="169">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="V214" s="169">
         <v>2</v>
       </c>
       <c r="W214" s="169">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="X214" s="169">
         <v>2</v>
@@ -67205,30 +67205,30 @@
         <v>3</v>
       </c>
       <c r="AA214" s="168">
-        <v>109</v>
-      </c>
-      <c r="AB214" s="168">
-        <v>118</v>
-      </c>
-      <c r="AC214" s="168">
-        <v>116</v>
-      </c>
-      <c r="AD214" s="168">
+        <v>107</v>
+      </c>
+      <c r="AB214" s="169">
+        <v>121</v>
+      </c>
+      <c r="AC214" s="169">
+        <v>117</v>
+      </c>
+      <c r="AD214" s="185">
         <v>7</v>
       </c>
-      <c r="AE214" s="168">
-        <v>6</v>
+      <c r="AE214" s="185">
+        <v>5</v>
       </c>
       <c r="AF214" s="169" t="s">
-        <v>731</v>
+        <v>734</v>
       </c>
       <c r="AG214" s="170" t="s">
-        <v>732</v>
+        <v>735</v>
       </c>
     </row>
     <row r="215" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="171" t="s">
-        <v>733</v>
+        <v>736</v>
       </c>
       <c r="B215" s="171">
         <v>60</v>
@@ -67237,31 +67237,31 @@
         <v>2</v>
       </c>
       <c r="D215" s="172">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E215" s="172">
         <v>26</v>
       </c>
       <c r="F215" s="172">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G215" s="172">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="H215" s="172">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="I215" s="172">
-        <v>112</v>
+        <v>160</v>
       </c>
       <c r="J215" s="172">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="K215" s="172">
-        <v>104</v>
+        <v>133</v>
       </c>
       <c r="L215" s="172">
-        <v>111</v>
+        <v>159</v>
       </c>
       <c r="M215" s="168">
         <v>0</v>
@@ -67272,26 +67272,26 @@
       <c r="O215" s="169">
         <v>0</v>
       </c>
-      <c r="P215" s="227">
-        <v>44746</v>
+      <c r="P215" s="177">
+        <v>0</v>
       </c>
       <c r="Q215" s="169">
         <v>0</v>
       </c>
       <c r="R215" s="169">
-        <v>91.67</v>
+        <v>100</v>
       </c>
       <c r="S215" s="169">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="T215" s="169">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U215" s="169">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="V215" s="169">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W215" s="169">
         <v>45</v>
@@ -67300,36 +67300,36 @@
         <v>2</v>
       </c>
       <c r="Y215" s="177">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="Z215" s="169">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AA215" s="168">
         <v>107</v>
       </c>
-      <c r="AB215" s="169">
-        <v>121</v>
-      </c>
-      <c r="AC215" s="169">
-        <v>117</v>
-      </c>
-      <c r="AD215" s="185">
+      <c r="AB215" s="177">
+        <v>131</v>
+      </c>
+      <c r="AC215" s="177">
+        <v>123</v>
+      </c>
+      <c r="AD215" s="168">
         <v>7</v>
       </c>
-      <c r="AE215" s="185">
-        <v>5</v>
-      </c>
-      <c r="AF215" s="169" t="s">
-        <v>734</v>
-      </c>
-      <c r="AG215" s="170" t="s">
-        <v>735</v>
+      <c r="AE215" s="168">
+        <v>7</v>
+      </c>
+      <c r="AF215" s="177" t="s">
+        <v>737</v>
+      </c>
+      <c r="AG215" s="207">
+        <v>5517984193</v>
       </c>
     </row>
     <row r="216" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="171" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="B216" s="171">
         <v>60</v>
@@ -67338,40 +67338,40 @@
         <v>2</v>
       </c>
       <c r="D216" s="172">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E216" s="172">
         <v>26</v>
       </c>
       <c r="F216" s="172">
-        <v>18</v>
+        <v>12.5</v>
       </c>
       <c r="G216" s="172">
-        <v>12</v>
+        <v>1.5</v>
       </c>
       <c r="H216" s="172">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="I216" s="172">
-        <v>160</v>
+        <v>112</v>
       </c>
       <c r="J216" s="172">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="K216" s="172">
-        <v>133</v>
+        <v>93</v>
       </c>
       <c r="L216" s="172">
-        <v>159</v>
+        <v>114</v>
       </c>
       <c r="M216" s="168">
         <v>0</v>
       </c>
       <c r="N216" s="169">
-        <v>0</v>
-      </c>
-      <c r="O216" s="169">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="O216" s="177">
+        <v>3</v>
       </c>
       <c r="P216" s="177">
         <v>0</v>
@@ -67380,28 +67380,28 @@
         <v>0</v>
       </c>
       <c r="R216" s="169">
-        <v>100</v>
-      </c>
-      <c r="S216" s="169">
-        <v>52</v>
+        <v>91.66</v>
+      </c>
+      <c r="S216" s="177">
+        <v>50</v>
       </c>
       <c r="T216" s="169">
         <v>3</v>
       </c>
-      <c r="U216" s="169">
-        <v>52</v>
-      </c>
-      <c r="V216" s="169">
-        <v>3</v>
+      <c r="U216" s="177">
+        <v>33</v>
+      </c>
+      <c r="V216" s="177">
+        <v>2</v>
       </c>
       <c r="W216" s="169">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="X216" s="169">
         <v>2</v>
       </c>
       <c r="Y216" s="177">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="Z216" s="169">
         <v>2</v>
@@ -67409,28 +67409,28 @@
       <c r="AA216" s="168">
         <v>107</v>
       </c>
-      <c r="AB216" s="177">
-        <v>131</v>
-      </c>
-      <c r="AC216" s="177">
-        <v>123</v>
-      </c>
-      <c r="AD216" s="168">
-        <v>7</v>
-      </c>
-      <c r="AE216" s="168">
-        <v>7</v>
+      <c r="AB216" s="169">
+        <v>105</v>
+      </c>
+      <c r="AC216" s="169">
+        <v>107</v>
+      </c>
+      <c r="AD216" s="173">
+        <v>6.9</v>
+      </c>
+      <c r="AE216" s="173">
+        <v>6.6</v>
       </c>
       <c r="AF216" s="177" t="s">
-        <v>737</v>
-      </c>
-      <c r="AG216" s="207">
-        <v>5517984193</v>
+        <v>739</v>
+      </c>
+      <c r="AG216" s="170" t="s">
+        <v>740</v>
       </c>
     </row>
     <row r="217" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A217" s="171" t="s">
-        <v>738</v>
+      <c r="A217" s="208" t="s">
+        <v>741</v>
       </c>
       <c r="B217" s="171">
         <v>60</v>
@@ -67445,25 +67445,25 @@
         <v>26</v>
       </c>
       <c r="F217" s="172">
-        <v>12.5</v>
+        <v>17</v>
       </c>
       <c r="G217" s="172">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="H217" s="172">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I217" s="172">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="J217" s="172">
-        <v>126</v>
+        <v>100</v>
       </c>
       <c r="K217" s="172">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L217" s="172">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="M217" s="168">
         <v>0</v>
@@ -67472,7 +67472,7 @@
         <v>1</v>
       </c>
       <c r="O217" s="177">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P217" s="177">
         <v>0</v>
@@ -67481,40 +67481,40 @@
         <v>0</v>
       </c>
       <c r="R217" s="169">
-        <v>91.66</v>
-      </c>
-      <c r="S217" s="177">
-        <v>50</v>
+        <v>91.3</v>
+      </c>
+      <c r="S217" s="169">
+        <v>42</v>
       </c>
       <c r="T217" s="169">
-        <v>3</v>
-      </c>
-      <c r="U217" s="177">
-        <v>33</v>
-      </c>
-      <c r="V217" s="177">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="U217" s="169">
+        <v>49</v>
+      </c>
+      <c r="V217" s="169">
+        <v>3</v>
       </c>
       <c r="W217" s="169">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="X217" s="169">
         <v>2</v>
       </c>
       <c r="Y217" s="177">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="Z217" s="169">
-        <v>2</v>
-      </c>
-      <c r="AA217" s="168">
-        <v>107</v>
-      </c>
-      <c r="AB217" s="169">
-        <v>105</v>
-      </c>
-      <c r="AC217" s="169">
-        <v>107</v>
+        <v>3</v>
+      </c>
+      <c r="AA217" s="212">
+        <v>109.62962962962963</v>
+      </c>
+      <c r="AB217" s="212">
+        <v>110.62962962962963</v>
+      </c>
+      <c r="AC217" s="212">
+        <v>112</v>
       </c>
       <c r="AD217" s="173">
         <v>6.9</v>
@@ -67523,15 +67523,15 @@
         <v>6.6</v>
       </c>
       <c r="AF217" s="177" t="s">
-        <v>739</v>
+        <v>742</v>
       </c>
       <c r="AG217" s="170" t="s">
-        <v>740</v>
+        <v>743</v>
       </c>
     </row>
     <row r="218" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A218" s="208" t="s">
-        <v>741</v>
+      <c r="A218" s="171" t="s">
+        <v>745</v>
       </c>
       <c r="B218" s="171">
         <v>60</v>
@@ -67540,31 +67540,31 @@
         <v>2</v>
       </c>
       <c r="D218" s="172">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E218" s="172">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F218" s="172">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G218" s="172">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H218" s="172">
-        <v>17</v>
+        <v>20.5</v>
       </c>
       <c r="I218" s="172">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="J218" s="172">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="K218" s="172">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="L218" s="172">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="M218" s="168">
         <v>0</v>
@@ -67572,8 +67572,8 @@
       <c r="N218" s="169">
         <v>1</v>
       </c>
-      <c r="O218" s="177">
-        <v>1</v>
+      <c r="O218" s="169">
+        <v>0</v>
       </c>
       <c r="P218" s="177">
         <v>0</v>
@@ -67582,57 +67582,57 @@
         <v>0</v>
       </c>
       <c r="R218" s="169">
-        <v>91.3</v>
+        <v>100</v>
       </c>
       <c r="S218" s="169">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="T218" s="169">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U218" s="169">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="V218" s="169">
         <v>3</v>
       </c>
       <c r="W218" s="169">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="X218" s="169">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y218" s="177">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="Z218" s="169">
         <v>3</v>
       </c>
-      <c r="AA218" s="212">
-        <v>109.62962962962963</v>
-      </c>
-      <c r="AB218" s="212">
-        <v>110.62962962962963</v>
-      </c>
-      <c r="AC218" s="212">
-        <v>112</v>
-      </c>
-      <c r="AD218" s="173">
-        <v>6.9</v>
-      </c>
-      <c r="AE218" s="173">
-        <v>6.6</v>
-      </c>
-      <c r="AF218" s="177" t="s">
-        <v>742</v>
+      <c r="AA218" s="168">
+        <v>111</v>
+      </c>
+      <c r="AB218" s="168">
+        <v>121</v>
+      </c>
+      <c r="AC218" s="168">
+        <v>119</v>
+      </c>
+      <c r="AD218" s="168">
+        <v>7</v>
+      </c>
+      <c r="AE218" s="168">
+        <v>7</v>
+      </c>
+      <c r="AF218" s="169" t="s">
+        <v>746</v>
       </c>
       <c r="AG218" s="170" t="s">
-        <v>743</v>
+        <v>747</v>
       </c>
     </row>
     <row r="219" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="171" t="s">
-        <v>745</v>
+        <v>748</v>
       </c>
       <c r="B219" s="171">
         <v>60</v>
@@ -67641,10 +67641,10 @@
         <v>2</v>
       </c>
       <c r="D219" s="172">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E219" s="172">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F219" s="172">
         <v>20</v>
@@ -67656,22 +67656,22 @@
         <v>20.5</v>
       </c>
       <c r="I219" s="172">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="J219" s="172">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="K219" s="172">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="L219" s="172">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="M219" s="168">
         <v>0</v>
       </c>
       <c r="N219" s="169">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O219" s="169">
         <v>0</v>
@@ -67686,54 +67686,54 @@
         <v>100</v>
       </c>
       <c r="S219" s="169">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="T219" s="169">
         <v>3</v>
       </c>
       <c r="U219" s="169">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="V219" s="169">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W219" s="169">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X219" s="169">
         <v>3</v>
       </c>
       <c r="Y219" s="177">
-        <v>48</v>
-      </c>
-      <c r="Z219" s="169">
-        <v>3</v>
-      </c>
-      <c r="AA219" s="168">
-        <v>111</v>
-      </c>
-      <c r="AB219" s="168">
-        <v>121</v>
-      </c>
-      <c r="AC219" s="168">
-        <v>119</v>
+        <v>42</v>
+      </c>
+      <c r="Z219" s="177">
+        <v>2</v>
+      </c>
+      <c r="AA219" s="169">
+        <v>105</v>
+      </c>
+      <c r="AB219" s="169">
+        <v>99</v>
+      </c>
+      <c r="AC219" s="169">
+        <v>102</v>
       </c>
       <c r="AD219" s="168">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AE219" s="168">
         <v>7</v>
       </c>
       <c r="AF219" s="169" t="s">
-        <v>746</v>
+        <v>749</v>
       </c>
       <c r="AG219" s="170" t="s">
-        <v>747</v>
+        <v>750</v>
       </c>
     </row>
     <row r="220" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="171" t="s">
-        <v>748</v>
+        <v>751</v>
       </c>
       <c r="B220" s="171">
         <v>60</v>
@@ -67742,37 +67742,37 @@
         <v>2</v>
       </c>
       <c r="D220" s="172">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="E220" s="172">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F220" s="172">
-        <v>20</v>
+        <v>16.5</v>
       </c>
       <c r="G220" s="172">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H220" s="172">
-        <v>20.5</v>
+        <v>17.5</v>
       </c>
       <c r="I220" s="172">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="J220" s="172">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="K220" s="172">
-        <v>127</v>
+        <v>84</v>
       </c>
       <c r="L220" s="172">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="M220" s="168">
         <v>0</v>
       </c>
       <c r="N220" s="169">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O220" s="169">
         <v>0</v>
@@ -67786,55 +67786,55 @@
       <c r="R220" s="169">
         <v>100</v>
       </c>
-      <c r="S220" s="169">
+      <c r="S220" s="177">
         <v>52</v>
       </c>
       <c r="T220" s="169">
         <v>3</v>
       </c>
       <c r="U220" s="169">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="V220" s="169">
         <v>2</v>
       </c>
       <c r="W220" s="169">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="X220" s="169">
-        <v>3</v>
-      </c>
-      <c r="Y220" s="177">
-        <v>42</v>
-      </c>
-      <c r="Z220" s="177">
+        <v>2</v>
+      </c>
+      <c r="Y220" s="169">
+        <v>37</v>
+      </c>
+      <c r="Z220" s="169">
         <v>2</v>
       </c>
       <c r="AA220" s="169">
-        <v>105</v>
-      </c>
-      <c r="AB220" s="169">
-        <v>99</v>
-      </c>
-      <c r="AC220" s="169">
-        <v>102</v>
-      </c>
-      <c r="AD220" s="168">
-        <v>8</v>
-      </c>
-      <c r="AE220" s="168">
-        <v>7</v>
+        <v>114</v>
+      </c>
+      <c r="AB220" s="177">
+        <v>104</v>
+      </c>
+      <c r="AC220" s="177">
+        <v>110</v>
+      </c>
+      <c r="AD220" s="173">
+        <v>6.9</v>
+      </c>
+      <c r="AE220" s="173">
+        <v>6.6</v>
       </c>
       <c r="AF220" s="169" t="s">
-        <v>749</v>
+        <v>752</v>
       </c>
       <c r="AG220" s="170" t="s">
-        <v>750</v>
+        <v>753</v>
       </c>
     </row>
     <row r="221" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="171" t="s">
-        <v>751</v>
+        <v>754</v>
       </c>
       <c r="B221" s="171">
         <v>60</v>
@@ -67843,99 +67843,99 @@
         <v>2</v>
       </c>
       <c r="D221" s="172">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="E221" s="172">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F221" s="172">
-        <v>16.5</v>
-      </c>
-      <c r="G221" s="172">
-        <v>1</v>
+        <v>25</v>
+      </c>
+      <c r="G221" s="171">
+        <v>0</v>
       </c>
       <c r="H221" s="172">
-        <v>17.5</v>
+        <v>25</v>
       </c>
       <c r="I221" s="172">
-        <v>127</v>
+        <v>144</v>
       </c>
       <c r="J221" s="172">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="K221" s="172">
-        <v>84</v>
+        <v>142</v>
       </c>
       <c r="L221" s="172">
-        <v>107</v>
-      </c>
-      <c r="M221" s="168">
-        <v>0</v>
-      </c>
-      <c r="N221" s="169">
-        <v>1</v>
-      </c>
-      <c r="O221" s="169">
+        <v>144</v>
+      </c>
+      <c r="M221" s="185">
+        <v>0</v>
+      </c>
+      <c r="N221" s="177">
+        <v>0</v>
+      </c>
+      <c r="O221" s="177">
         <v>0</v>
       </c>
       <c r="P221" s="177">
         <v>0</v>
       </c>
-      <c r="Q221" s="169">
+      <c r="Q221" s="177">
         <v>0</v>
       </c>
       <c r="R221" s="169">
         <v>100</v>
       </c>
       <c r="S221" s="177">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="T221" s="169">
-        <v>3</v>
-      </c>
-      <c r="U221" s="169">
-        <v>36</v>
+        <v>2</v>
+      </c>
+      <c r="U221" s="177">
+        <v>42</v>
       </c>
       <c r="V221" s="169">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W221" s="169">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="X221" s="169">
-        <v>2</v>
-      </c>
-      <c r="Y221" s="169">
-        <v>37</v>
+        <v>3</v>
+      </c>
+      <c r="Y221" s="177">
+        <v>53</v>
       </c>
       <c r="Z221" s="169">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA221" s="169">
-        <v>114</v>
-      </c>
-      <c r="AB221" s="177">
-        <v>104</v>
-      </c>
-      <c r="AC221" s="177">
-        <v>110</v>
-      </c>
-      <c r="AD221" s="173">
-        <v>6.9</v>
-      </c>
-      <c r="AE221" s="173">
-        <v>6.6</v>
-      </c>
-      <c r="AF221" s="169" t="s">
-        <v>752</v>
+        <v>107</v>
+      </c>
+      <c r="AB221" s="169">
+        <v>102</v>
+      </c>
+      <c r="AC221" s="169">
+        <v>105</v>
+      </c>
+      <c r="AD221" s="168">
+        <v>6</v>
+      </c>
+      <c r="AE221" s="168">
+        <v>6</v>
+      </c>
+      <c r="AF221" s="177" t="s">
+        <v>755</v>
       </c>
       <c r="AG221" s="170" t="s">
-        <v>753</v>
+        <v>805</v>
       </c>
     </row>
     <row r="222" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="171" t="s">
-        <v>754</v>
+        <v>757</v>
       </c>
       <c r="B222" s="171">
         <v>60</v>
@@ -67944,99 +67944,99 @@
         <v>2</v>
       </c>
       <c r="D222" s="172">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E222" s="172">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F222" s="172">
-        <v>25</v>
-      </c>
-      <c r="G222" s="171">
+        <v>16</v>
+      </c>
+      <c r="G222" s="172">
         <v>0</v>
       </c>
       <c r="H222" s="172">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="I222" s="172">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="J222" s="172">
-        <v>114</v>
+        <v>86</v>
       </c>
       <c r="K222" s="172">
-        <v>142</v>
+        <v>95</v>
       </c>
       <c r="L222" s="172">
-        <v>144</v>
-      </c>
-      <c r="M222" s="185">
-        <v>0</v>
-      </c>
-      <c r="N222" s="177">
-        <v>0</v>
-      </c>
-      <c r="O222" s="177">
+        <v>99</v>
+      </c>
+      <c r="M222" s="168">
+        <v>0</v>
+      </c>
+      <c r="N222" s="169">
+        <v>0</v>
+      </c>
+      <c r="O222" s="169">
         <v>0</v>
       </c>
       <c r="P222" s="177">
         <v>0</v>
       </c>
-      <c r="Q222" s="177">
+      <c r="Q222" s="169">
         <v>0</v>
       </c>
       <c r="R222" s="169">
         <v>100</v>
       </c>
       <c r="S222" s="177">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="T222" s="169">
         <v>2</v>
       </c>
       <c r="U222" s="177">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="V222" s="169">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W222" s="169">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="X222" s="169">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Y222" s="177">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="Z222" s="169">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AA222" s="169">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="AB222" s="169">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="AC222" s="169">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="AD222" s="168">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AE222" s="168">
-        <v>6</v>
-      </c>
-      <c r="AF222" s="177" t="s">
-        <v>755</v>
+        <v>7</v>
+      </c>
+      <c r="AF222" s="169" t="s">
+        <v>758</v>
       </c>
       <c r="AG222" s="170" t="s">
-        <v>805</v>
+        <v>759</v>
       </c>
     </row>
     <row r="223" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="171" t="s">
-        <v>757</v>
+        <v>760</v>
       </c>
       <c r="B223" s="171">
         <v>60</v>
@@ -68045,99 +68045,99 @@
         <v>2</v>
       </c>
       <c r="D223" s="172">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E223" s="172">
         <v>27</v>
       </c>
       <c r="F223" s="172">
-        <v>16</v>
+        <v>21.5</v>
       </c>
       <c r="G223" s="172">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H223" s="172">
-        <v>16</v>
+        <v>26.5</v>
       </c>
       <c r="I223" s="172">
-        <v>117</v>
+        <v>148</v>
       </c>
       <c r="J223" s="172">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="K223" s="172">
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="L223" s="172">
+        <v>139</v>
+      </c>
+      <c r="M223" s="168">
+        <v>0</v>
+      </c>
+      <c r="N223" s="169">
+        <v>0</v>
+      </c>
+      <c r="O223" s="169">
+        <v>0</v>
+      </c>
+      <c r="P223" s="177">
+        <v>0</v>
+      </c>
+      <c r="Q223" s="169">
+        <v>0</v>
+      </c>
+      <c r="R223" s="169">
+        <v>65.209999999999994</v>
+      </c>
+      <c r="S223" s="177">
+        <v>41</v>
+      </c>
+      <c r="T223" s="177">
+        <v>2</v>
+      </c>
+      <c r="U223" s="177">
+        <v>49</v>
+      </c>
+      <c r="V223" s="177">
+        <v>3</v>
+      </c>
+      <c r="W223" s="177">
+        <v>46</v>
+      </c>
+      <c r="X223" s="177">
+        <v>2</v>
+      </c>
+      <c r="Y223" s="177">
+        <v>42</v>
+      </c>
+      <c r="Z223" s="177">
+        <v>2</v>
+      </c>
+      <c r="AA223" s="177">
+        <v>114</v>
+      </c>
+      <c r="AB223" s="177">
         <v>99</v>
       </c>
-      <c r="M223" s="168">
-        <v>0</v>
-      </c>
-      <c r="N223" s="169">
-        <v>0</v>
-      </c>
-      <c r="O223" s="169">
-        <v>0</v>
-      </c>
-      <c r="P223" s="177">
-        <v>0</v>
-      </c>
-      <c r="Q223" s="169">
-        <v>0</v>
-      </c>
-      <c r="R223" s="169">
-        <v>100</v>
-      </c>
-      <c r="S223" s="177">
-        <v>39</v>
-      </c>
-      <c r="T223" s="169">
-        <v>2</v>
-      </c>
-      <c r="U223" s="177">
-        <v>44</v>
-      </c>
-      <c r="V223" s="169">
-        <v>2</v>
-      </c>
-      <c r="W223" s="169">
-        <v>26</v>
-      </c>
-      <c r="X223" s="169">
-        <v>1</v>
-      </c>
-      <c r="Y223" s="177">
-        <v>32</v>
-      </c>
-      <c r="Z223" s="169">
-        <v>2</v>
-      </c>
-      <c r="AA223" s="169">
-        <v>84</v>
-      </c>
-      <c r="AB223" s="169">
-        <v>96</v>
-      </c>
-      <c r="AC223" s="169">
-        <v>88</v>
-      </c>
-      <c r="AD223" s="168">
-        <v>7</v>
-      </c>
-      <c r="AE223" s="168">
-        <v>7</v>
+      <c r="AC223" s="177">
+        <v>108</v>
+      </c>
+      <c r="AD223" s="185">
+        <v>8</v>
+      </c>
+      <c r="AE223" s="185">
+        <v>8</v>
       </c>
       <c r="AF223" s="169" t="s">
-        <v>758</v>
+        <v>761</v>
       </c>
       <c r="AG223" s="170" t="s">
-        <v>759</v>
+        <v>762</v>
       </c>
     </row>
     <row r="224" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="171" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="B224" s="171">
         <v>60</v>
@@ -68145,100 +68145,100 @@
       <c r="C224" s="171">
         <v>2</v>
       </c>
-      <c r="D224" s="172">
+      <c r="D224" s="171">
         <v>60</v>
       </c>
-      <c r="E224" s="172">
+      <c r="E224" s="171">
         <v>27</v>
       </c>
       <c r="F224" s="172">
-        <v>21.5</v>
+        <v>19</v>
       </c>
       <c r="G224" s="172">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H224" s="172">
-        <v>26.5</v>
+        <v>19</v>
       </c>
       <c r="I224" s="172">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="J224" s="172">
+        <v>143</v>
+      </c>
+      <c r="K224" s="172">
+        <v>126</v>
+      </c>
+      <c r="L224" s="172">
+        <v>141</v>
+      </c>
+      <c r="M224" s="168">
+        <v>0</v>
+      </c>
+      <c r="N224" s="169">
+        <v>0</v>
+      </c>
+      <c r="O224" s="177">
+        <v>0</v>
+      </c>
+      <c r="P224" s="227">
+        <v>44754</v>
+      </c>
+      <c r="Q224" s="169">
+        <v>0</v>
+      </c>
+      <c r="R224" s="169">
+        <v>100</v>
+      </c>
+      <c r="S224" s="177">
+        <v>49</v>
+      </c>
+      <c r="T224" s="177">
+        <v>3</v>
+      </c>
+      <c r="U224" s="177">
+        <v>43</v>
+      </c>
+      <c r="V224" s="177">
+        <v>2</v>
+      </c>
+      <c r="W224" s="177">
+        <v>50</v>
+      </c>
+      <c r="X224" s="177">
+        <v>3</v>
+      </c>
+      <c r="Y224" s="177">
+        <v>50</v>
+      </c>
+      <c r="Z224" s="177">
+        <v>3</v>
+      </c>
+      <c r="AA224" s="177">
+        <v>111</v>
+      </c>
+      <c r="AB224" s="177">
+        <v>115</v>
+      </c>
+      <c r="AC224" s="177">
         <v>116</v>
       </c>
-      <c r="K224" s="172">
-        <v>125</v>
-      </c>
-      <c r="L224" s="172">
-        <v>139</v>
-      </c>
-      <c r="M224" s="168">
-        <v>0</v>
-      </c>
-      <c r="N224" s="169">
-        <v>0</v>
-      </c>
-      <c r="O224" s="169">
-        <v>0</v>
-      </c>
-      <c r="P224" s="177">
-        <v>0</v>
-      </c>
-      <c r="Q224" s="169">
-        <v>0</v>
-      </c>
-      <c r="R224" s="169">
-        <v>65.209999999999994</v>
-      </c>
-      <c r="S224" s="177">
-        <v>41</v>
-      </c>
-      <c r="T224" s="177">
-        <v>2</v>
-      </c>
-      <c r="U224" s="177">
-        <v>49</v>
-      </c>
-      <c r="V224" s="177">
-        <v>3</v>
-      </c>
-      <c r="W224" s="177">
-        <v>46</v>
-      </c>
-      <c r="X224" s="177">
-        <v>2</v>
-      </c>
-      <c r="Y224" s="177">
-        <v>42</v>
-      </c>
-      <c r="Z224" s="177">
-        <v>2</v>
-      </c>
-      <c r="AA224" s="177">
-        <v>114</v>
-      </c>
-      <c r="AB224" s="177">
-        <v>99</v>
-      </c>
-      <c r="AC224" s="177">
-        <v>108</v>
-      </c>
       <c r="AD224" s="185">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AE224" s="185">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="AF224" s="169" t="s">
-        <v>761</v>
+        <v>764</v>
       </c>
       <c r="AG224" s="170" t="s">
-        <v>762</v>
+        <v>765</v>
       </c>
     </row>
     <row r="225" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A225" s="171" t="s">
-        <v>763</v>
+      <c r="A225" s="203" t="s">
+        <v>766</v>
       </c>
       <c r="B225" s="171">
         <v>60</v>
@@ -68246,201 +68246,201 @@
       <c r="C225" s="171">
         <v>2</v>
       </c>
-      <c r="D225" s="171">
-        <v>60</v>
-      </c>
-      <c r="E225" s="171">
+      <c r="D225" s="172">
+        <v>67</v>
+      </c>
+      <c r="E225" s="172">
+        <v>26</v>
+      </c>
+      <c r="F225" s="172">
+        <v>12</v>
+      </c>
+      <c r="G225" s="172">
+        <v>10</v>
+      </c>
+      <c r="H225" s="172">
+        <v>22</v>
+      </c>
+      <c r="I225" s="172">
+        <v>137</v>
+      </c>
+      <c r="J225" s="172">
+        <v>89</v>
+      </c>
+      <c r="K225" s="172">
+        <v>89</v>
+      </c>
+      <c r="L225" s="172">
+        <v>107</v>
+      </c>
+      <c r="M225" s="185">
+        <v>0</v>
+      </c>
+      <c r="N225" s="177">
+        <v>0</v>
+      </c>
+      <c r="O225" s="177">
+        <v>0</v>
+      </c>
+      <c r="P225" s="177">
+        <v>0</v>
+      </c>
+      <c r="Q225" s="177">
+        <v>0</v>
+      </c>
+      <c r="R225" s="177">
+        <v>100</v>
+      </c>
+      <c r="S225" s="177">
+        <v>48</v>
+      </c>
+      <c r="T225" s="177">
+        <v>3</v>
+      </c>
+      <c r="U225" s="177">
+        <v>50</v>
+      </c>
+      <c r="V225" s="177">
+        <v>3</v>
+      </c>
+      <c r="W225" s="177">
+        <v>47</v>
+      </c>
+      <c r="X225" s="177">
+        <v>3</v>
+      </c>
+      <c r="Y225" s="177">
+        <v>45</v>
+      </c>
+      <c r="Z225" s="177">
+        <v>3</v>
+      </c>
+      <c r="AA225" s="177">
+        <v>101</v>
+      </c>
+      <c r="AB225" s="177">
+        <v>109</v>
+      </c>
+      <c r="AC225" s="177">
+        <v>106</v>
+      </c>
+      <c r="AD225" s="185">
+        <v>9</v>
+      </c>
+      <c r="AE225" s="185">
+        <v>8</v>
+      </c>
+      <c r="AF225" s="177" t="s">
+        <v>767</v>
+      </c>
+      <c r="AG225" s="170">
+        <v>5611745443</v>
+      </c>
+    </row>
+    <row r="226" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A226" s="171" t="s">
+        <v>768</v>
+      </c>
+      <c r="B226" s="171">
+        <v>70</v>
+      </c>
+      <c r="C226" s="171">
+        <v>1</v>
+      </c>
+      <c r="D226" s="172">
+        <v>72</v>
+      </c>
+      <c r="E226" s="172">
         <v>27</v>
       </c>
-      <c r="F225" s="172">
-        <v>19</v>
-      </c>
-      <c r="G225" s="172">
-        <v>0</v>
-      </c>
-      <c r="H225" s="172">
-        <v>19</v>
-      </c>
-      <c r="I225" s="172">
+      <c r="F226" s="172">
+        <v>16.5</v>
+      </c>
+      <c r="G226" s="172">
+        <v>0.5</v>
+      </c>
+      <c r="H226" s="215">
+        <v>17</v>
+      </c>
+      <c r="I226" s="172">
         <v>124</v>
       </c>
-      <c r="J225" s="172">
-        <v>143</v>
-      </c>
-      <c r="K225" s="172">
-        <v>126</v>
-      </c>
-      <c r="L225" s="172">
-        <v>141</v>
-      </c>
-      <c r="M225" s="168">
-        <v>0</v>
-      </c>
-      <c r="N225" s="169">
-        <v>0</v>
-      </c>
-      <c r="O225" s="177">
-        <v>0</v>
-      </c>
-      <c r="P225" s="227">
-        <v>44754</v>
-      </c>
-      <c r="Q225" s="169">
-        <v>0</v>
-      </c>
-      <c r="R225" s="169">
+      <c r="J226" s="172">
+        <v>155</v>
+      </c>
+      <c r="K226" s="172">
+        <v>107</v>
+      </c>
+      <c r="L226" s="172">
+        <v>138</v>
+      </c>
+      <c r="M226" s="168">
+        <v>0</v>
+      </c>
+      <c r="N226" s="169">
+        <v>0</v>
+      </c>
+      <c r="O226" s="169">
+        <v>0</v>
+      </c>
+      <c r="P226" s="177">
+        <v>0</v>
+      </c>
+      <c r="Q226" s="169">
+        <v>0</v>
+      </c>
+      <c r="R226" s="169">
         <v>100</v>
       </c>
-      <c r="S225" s="177">
-        <v>49</v>
-      </c>
-      <c r="T225" s="177">
-        <v>3</v>
-      </c>
-      <c r="U225" s="177">
-        <v>43</v>
-      </c>
-      <c r="V225" s="177">
-        <v>2</v>
-      </c>
-      <c r="W225" s="177">
-        <v>50</v>
-      </c>
-      <c r="X225" s="177">
-        <v>3</v>
-      </c>
-      <c r="Y225" s="177">
-        <v>50</v>
-      </c>
-      <c r="Z225" s="177">
-        <v>3</v>
-      </c>
-      <c r="AA225" s="177">
-        <v>111</v>
-      </c>
-      <c r="AB225" s="177">
-        <v>115</v>
-      </c>
-      <c r="AC225" s="177">
-        <v>116</v>
-      </c>
-      <c r="AD225" s="185">
-        <v>7</v>
-      </c>
-      <c r="AE225" s="185">
-        <v>6</v>
-      </c>
-      <c r="AF225" s="169" t="s">
-        <v>764</v>
-      </c>
-      <c r="AG225" s="170" t="s">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="226" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A226" s="203" t="s">
-        <v>766</v>
-      </c>
-      <c r="B226" s="171">
-        <v>60</v>
-      </c>
-      <c r="C226" s="171">
-        <v>2</v>
-      </c>
-      <c r="D226" s="172">
-        <v>67</v>
-      </c>
-      <c r="E226" s="172">
-        <v>26</v>
-      </c>
-      <c r="F226" s="172">
-        <v>12</v>
-      </c>
-      <c r="G226" s="172">
-        <v>10</v>
-      </c>
-      <c r="H226" s="172">
-        <v>22</v>
-      </c>
-      <c r="I226" s="172">
-        <v>137</v>
-      </c>
-      <c r="J226" s="172">
-        <v>89</v>
-      </c>
-      <c r="K226" s="172">
-        <v>89</v>
-      </c>
-      <c r="L226" s="172">
-        <v>107</v>
-      </c>
-      <c r="M226" s="185">
-        <v>0</v>
-      </c>
-      <c r="N226" s="177">
-        <v>0</v>
-      </c>
-      <c r="O226" s="177">
-        <v>0</v>
-      </c>
-      <c r="P226" s="177">
-        <v>0</v>
-      </c>
-      <c r="Q226" s="177">
-        <v>0</v>
-      </c>
-      <c r="R226" s="177">
-        <v>100</v>
-      </c>
-      <c r="S226" s="177">
-        <v>48</v>
-      </c>
-      <c r="T226" s="177">
-        <v>3</v>
-      </c>
-      <c r="U226" s="177">
-        <v>50</v>
-      </c>
-      <c r="V226" s="177">
-        <v>3</v>
-      </c>
-      <c r="W226" s="177">
+      <c r="S226" s="169">
+        <v>45</v>
+      </c>
+      <c r="T226" s="169">
+        <v>3</v>
+      </c>
+      <c r="U226" s="169">
+        <v>45</v>
+      </c>
+      <c r="V226" s="169">
+        <v>3</v>
+      </c>
+      <c r="W226" s="169">
         <v>47</v>
       </c>
-      <c r="X226" s="177">
+      <c r="X226" s="169">
         <v>3</v>
       </c>
       <c r="Y226" s="177">
-        <v>45</v>
-      </c>
-      <c r="Z226" s="177">
-        <v>3</v>
-      </c>
-      <c r="AA226" s="177">
-        <v>101</v>
-      </c>
-      <c r="AB226" s="177">
-        <v>109</v>
-      </c>
-      <c r="AC226" s="177">
+        <v>44</v>
+      </c>
+      <c r="Z226" s="169">
+        <v>3</v>
+      </c>
+      <c r="AA226" s="169">
         <v>106</v>
       </c>
-      <c r="AD226" s="185">
-        <v>9</v>
-      </c>
-      <c r="AE226" s="185">
-        <v>8</v>
-      </c>
-      <c r="AF226" s="177" t="s">
-        <v>767</v>
-      </c>
-      <c r="AG226" s="170">
-        <v>5611745443</v>
+      <c r="AB226" s="169">
+        <v>112</v>
+      </c>
+      <c r="AC226" s="169">
+        <v>110</v>
+      </c>
+      <c r="AD226" s="173">
+        <v>6.9</v>
+      </c>
+      <c r="AE226" s="173">
+        <v>7.1</v>
+      </c>
+      <c r="AF226" s="169" t="s">
+        <v>769</v>
+      </c>
+      <c r="AG226" s="170" t="s">
+        <v>770</v>
       </c>
     </row>
     <row r="227" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="171" t="s">
-        <v>768</v>
+        <v>771</v>
       </c>
       <c r="B227" s="171">
         <v>70</v>
@@ -68449,28 +68449,28 @@
         <v>1</v>
       </c>
       <c r="D227" s="172">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="E227" s="172">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F227" s="172">
-        <v>16.5</v>
+        <v>20.5</v>
       </c>
       <c r="G227" s="172">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H227" s="215">
-        <v>17</v>
+        <v>20.5</v>
       </c>
       <c r="I227" s="172">
-        <v>124</v>
+        <v>139</v>
       </c>
       <c r="J227" s="172">
-        <v>155</v>
+        <v>97</v>
       </c>
       <c r="K227" s="172">
-        <v>107</v>
+        <v>150</v>
       </c>
       <c r="L227" s="172">
         <v>138</v>
@@ -68484,47 +68484,47 @@
       <c r="O227" s="169">
         <v>0</v>
       </c>
-      <c r="P227" s="177">
-        <v>0</v>
+      <c r="P227" s="227">
+        <v>44176</v>
       </c>
       <c r="Q227" s="169">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R227" s="169">
-        <v>100</v>
+        <v>47.37</v>
       </c>
       <c r="S227" s="169">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="T227" s="169">
         <v>3</v>
       </c>
       <c r="U227" s="169">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="V227" s="169">
         <v>3</v>
       </c>
       <c r="W227" s="169">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="X227" s="169">
         <v>3</v>
       </c>
       <c r="Y227" s="177">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="Z227" s="169">
         <v>3</v>
       </c>
       <c r="AA227" s="169">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="AB227" s="169">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="AC227" s="169">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="AD227" s="173">
         <v>6.9</v>
@@ -68533,15 +68533,15 @@
         <v>7.1</v>
       </c>
       <c r="AF227" s="169" t="s">
-        <v>769</v>
+        <v>772</v>
       </c>
       <c r="AG227" s="170" t="s">
-        <v>770</v>
+        <v>773</v>
       </c>
     </row>
     <row r="228" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="171" t="s">
-        <v>771</v>
+        <v>774</v>
       </c>
       <c r="B228" s="171">
         <v>70</v>
@@ -68550,99 +68550,99 @@
         <v>1</v>
       </c>
       <c r="D228" s="172">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E228" s="172">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F228" s="172">
-        <v>20.5</v>
+        <v>18</v>
       </c>
       <c r="G228" s="172">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H228" s="215">
-        <v>20.5</v>
+        <v>19</v>
       </c>
       <c r="I228" s="172">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="J228" s="172">
-        <v>97</v>
+        <v>144</v>
       </c>
       <c r="K228" s="172">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="L228" s="172">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="M228" s="168">
         <v>0</v>
       </c>
-      <c r="N228" s="169">
-        <v>0</v>
-      </c>
-      <c r="O228" s="169">
-        <v>0</v>
-      </c>
-      <c r="P228" s="227">
-        <v>44176</v>
-      </c>
-      <c r="Q228" s="169">
+      <c r="N228" s="168">
+        <v>0</v>
+      </c>
+      <c r="O228" s="168">
+        <v>0</v>
+      </c>
+      <c r="P228" s="185">
+        <v>0</v>
+      </c>
+      <c r="Q228" s="168">
+        <v>0</v>
+      </c>
+      <c r="R228" s="168">
+        <v>41.18</v>
+      </c>
+      <c r="S228" s="169">
+        <v>45</v>
+      </c>
+      <c r="T228" s="169">
+        <v>3</v>
+      </c>
+      <c r="U228" s="169">
+        <v>45</v>
+      </c>
+      <c r="V228" s="169">
+        <v>3</v>
+      </c>
+      <c r="W228" s="169">
+        <v>50</v>
+      </c>
+      <c r="X228" s="169">
+        <v>3</v>
+      </c>
+      <c r="Y228" s="177">
+        <v>43</v>
+      </c>
+      <c r="Z228" s="169">
+        <v>3</v>
+      </c>
+      <c r="AA228" s="169">
+        <v>120</v>
+      </c>
+      <c r="AB228" s="169">
+        <v>131</v>
+      </c>
+      <c r="AC228" s="169">
+        <v>133</v>
+      </c>
+      <c r="AD228" s="168">
+        <v>7</v>
+      </c>
+      <c r="AE228" s="168">
         <v>8</v>
       </c>
-      <c r="R228" s="169">
-        <v>47.37</v>
-      </c>
-      <c r="S228" s="169">
-        <v>51</v>
-      </c>
-      <c r="T228" s="169">
-        <v>3</v>
-      </c>
-      <c r="U228" s="169">
-        <v>52</v>
-      </c>
-      <c r="V228" s="169">
-        <v>3</v>
-      </c>
-      <c r="W228" s="169">
-        <v>55</v>
-      </c>
-      <c r="X228" s="169">
-        <v>3</v>
-      </c>
-      <c r="Y228" s="177">
-        <v>55</v>
-      </c>
-      <c r="Z228" s="169">
-        <v>3</v>
-      </c>
-      <c r="AA228" s="169">
-        <v>116</v>
-      </c>
-      <c r="AB228" s="169">
-        <v>122</v>
-      </c>
-      <c r="AC228" s="169">
-        <v>124</v>
-      </c>
-      <c r="AD228" s="173">
-        <v>6.9</v>
-      </c>
-      <c r="AE228" s="173">
-        <v>7.1</v>
-      </c>
       <c r="AF228" s="169" t="s">
-        <v>772</v>
+        <v>775</v>
       </c>
       <c r="AG228" s="170" t="s">
-        <v>773</v>
+        <v>776</v>
       </c>
     </row>
     <row r="229" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="171" t="s">
-        <v>774</v>
+        <v>777</v>
       </c>
       <c r="B229" s="171">
         <v>70</v>
@@ -68651,200 +68651,200 @@
         <v>1</v>
       </c>
       <c r="D229" s="172">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E229" s="172">
         <v>27</v>
       </c>
       <c r="F229" s="172">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G229" s="172">
         <v>1</v>
       </c>
       <c r="H229" s="215">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I229" s="172">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="J229" s="172">
         <v>144</v>
       </c>
       <c r="K229" s="172">
-        <v>131</v>
+        <v>94</v>
       </c>
       <c r="L229" s="172">
-        <v>147</v>
-      </c>
-      <c r="M229" s="168">
-        <v>0</v>
-      </c>
-      <c r="N229" s="168">
-        <v>0</v>
-      </c>
-      <c r="O229" s="168">
-        <v>0</v>
-      </c>
-      <c r="P229" s="185">
-        <v>0</v>
-      </c>
-      <c r="Q229" s="168">
-        <v>0</v>
-      </c>
-      <c r="R229" s="168">
-        <v>41.18</v>
-      </c>
-      <c r="S229" s="169">
-        <v>45</v>
-      </c>
-      <c r="T229" s="169">
-        <v>3</v>
-      </c>
-      <c r="U229" s="169">
-        <v>45</v>
-      </c>
-      <c r="V229" s="169">
-        <v>3</v>
-      </c>
-      <c r="W229" s="169">
-        <v>50</v>
-      </c>
-      <c r="X229" s="169">
-        <v>3</v>
+        <v>127</v>
+      </c>
+      <c r="M229" s="185">
+        <v>0</v>
+      </c>
+      <c r="N229" s="185">
+        <v>0</v>
+      </c>
+      <c r="O229" s="185">
+        <v>0</v>
+      </c>
+      <c r="P229" s="185" t="s">
+        <v>778</v>
+      </c>
+      <c r="Q229" s="185">
+        <v>0</v>
+      </c>
+      <c r="R229" s="185">
+        <v>90</v>
+      </c>
+      <c r="S229" s="177">
+        <v>44</v>
+      </c>
+      <c r="T229" s="177">
+        <v>2</v>
+      </c>
+      <c r="U229" s="177">
+        <v>43</v>
+      </c>
+      <c r="V229" s="177">
+        <v>2</v>
+      </c>
+      <c r="W229" s="177">
+        <v>44</v>
+      </c>
+      <c r="X229" s="177">
+        <v>2</v>
       </c>
       <c r="Y229" s="177">
         <v>43</v>
       </c>
-      <c r="Z229" s="169">
-        <v>3</v>
-      </c>
-      <c r="AA229" s="169">
+      <c r="Z229" s="177">
+        <v>3</v>
+      </c>
+      <c r="AA229" s="177">
+        <v>116</v>
+      </c>
+      <c r="AB229" s="177">
+        <v>117</v>
+      </c>
+      <c r="AC229" s="177">
         <v>120</v>
       </c>
-      <c r="AB229" s="169">
-        <v>131</v>
-      </c>
-      <c r="AC229" s="169">
-        <v>133</v>
-      </c>
-      <c r="AD229" s="168">
+      <c r="AD229" s="185">
+        <v>8</v>
+      </c>
+      <c r="AE229" s="185">
         <v>7</v>
       </c>
-      <c r="AE229" s="168">
-        <v>8</v>
-      </c>
-      <c r="AF229" s="169" t="s">
-        <v>775</v>
+      <c r="AF229" s="177" t="s">
+        <v>779</v>
       </c>
       <c r="AG229" s="170" t="s">
-        <v>776</v>
+        <v>780</v>
       </c>
     </row>
     <row r="230" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="171" t="s">
-        <v>777</v>
+        <v>785</v>
       </c>
       <c r="B230" s="171">
         <v>70</v>
       </c>
       <c r="C230" s="171">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D230" s="172">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E230" s="172">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F230" s="172">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G230" s="172">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H230" s="215">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="I230" s="172">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="J230" s="172">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="K230" s="172">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="L230" s="172">
-        <v>127</v>
-      </c>
-      <c r="M230" s="185">
-        <v>0</v>
-      </c>
-      <c r="N230" s="185">
-        <v>0</v>
-      </c>
-      <c r="O230" s="185">
-        <v>0</v>
-      </c>
-      <c r="P230" s="185" t="s">
-        <v>778</v>
-      </c>
-      <c r="Q230" s="185">
-        <v>0</v>
-      </c>
-      <c r="R230" s="185">
-        <v>90</v>
-      </c>
-      <c r="S230" s="177">
-        <v>44</v>
-      </c>
-      <c r="T230" s="177">
-        <v>2</v>
-      </c>
-      <c r="U230" s="177">
-        <v>43</v>
-      </c>
-      <c r="V230" s="177">
-        <v>2</v>
-      </c>
-      <c r="W230" s="177">
-        <v>44</v>
-      </c>
-      <c r="X230" s="177">
+        <v>151</v>
+      </c>
+      <c r="M230" s="168">
+        <v>0</v>
+      </c>
+      <c r="N230" s="169">
+        <v>0</v>
+      </c>
+      <c r="O230" s="169">
+        <v>0</v>
+      </c>
+      <c r="P230" s="177">
+        <v>0</v>
+      </c>
+      <c r="Q230" s="169">
+        <v>0</v>
+      </c>
+      <c r="R230" s="168">
+        <v>100</v>
+      </c>
+      <c r="S230" s="169">
+        <v>47</v>
+      </c>
+      <c r="T230" s="169">
+        <v>3</v>
+      </c>
+      <c r="U230" s="169">
+        <v>36</v>
+      </c>
+      <c r="V230" s="169">
+        <v>2</v>
+      </c>
+      <c r="W230" s="169">
+        <v>42</v>
+      </c>
+      <c r="X230" s="169">
         <v>2</v>
       </c>
       <c r="Y230" s="177">
-        <v>43</v>
-      </c>
-      <c r="Z230" s="177">
-        <v>3</v>
-      </c>
-      <c r="AA230" s="177">
-        <v>116</v>
-      </c>
-      <c r="AB230" s="177">
-        <v>117</v>
-      </c>
-      <c r="AC230" s="177">
+        <v>47</v>
+      </c>
+      <c r="Z230" s="169">
+        <v>3</v>
+      </c>
+      <c r="AA230" s="169">
         <v>120</v>
       </c>
-      <c r="AD230" s="185">
-        <v>8</v>
-      </c>
-      <c r="AE230" s="185">
-        <v>7</v>
-      </c>
-      <c r="AF230" s="177" t="s">
-        <v>779</v>
+      <c r="AB230" s="169">
+        <v>112</v>
+      </c>
+      <c r="AC230" s="169">
+        <v>119</v>
+      </c>
+      <c r="AD230" s="173">
+        <v>6.9</v>
+      </c>
+      <c r="AE230" s="173">
+        <v>6.6</v>
+      </c>
+      <c r="AF230" s="169" t="s">
+        <v>786</v>
       </c>
       <c r="AG230" s="170" t="s">
-        <v>780</v>
+        <v>787</v>
       </c>
     </row>
     <row r="231" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="171" t="s">
-        <v>785</v>
+        <v>788</v>
       </c>
       <c r="B231" s="171">
         <v>70</v>
@@ -68853,31 +68853,31 @@
         <v>2</v>
       </c>
       <c r="D231" s="172">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E231" s="172">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F231" s="172">
-        <v>21</v>
+        <v>16.5</v>
       </c>
       <c r="G231" s="172">
         <v>0</v>
       </c>
       <c r="H231" s="215">
-        <v>21</v>
+        <v>16.5</v>
       </c>
       <c r="I231" s="172">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="J231" s="172">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="K231" s="172">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="L231" s="172">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="M231" s="168">
         <v>0</v>
@@ -68898,37 +68898,37 @@
         <v>100</v>
       </c>
       <c r="S231" s="169">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="T231" s="169">
         <v>3</v>
       </c>
       <c r="U231" s="169">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="V231" s="169">
         <v>2</v>
       </c>
       <c r="W231" s="169">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="X231" s="169">
         <v>2</v>
       </c>
       <c r="Y231" s="177">
-        <v>47</v>
-      </c>
-      <c r="Z231" s="169">
-        <v>3</v>
+        <v>39</v>
+      </c>
+      <c r="Z231" s="177">
+        <v>2</v>
       </c>
       <c r="AA231" s="169">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="AB231" s="169">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="AC231" s="169">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="AD231" s="173">
         <v>6.9</v>
@@ -68937,15 +68937,15 @@
         <v>6.6</v>
       </c>
       <c r="AF231" s="169" t="s">
-        <v>786</v>
+        <v>789</v>
       </c>
       <c r="AG231" s="170" t="s">
-        <v>787</v>
+        <v>790</v>
       </c>
     </row>
     <row r="232" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="171" t="s">
-        <v>788</v>
+        <v>791</v>
       </c>
       <c r="B232" s="171">
         <v>70</v>
@@ -68957,28 +68957,28 @@
         <v>70</v>
       </c>
       <c r="E232" s="172">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F232" s="172">
         <v>16.5</v>
       </c>
       <c r="G232" s="172">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="H232" s="215">
-        <v>16.5</v>
+        <v>19</v>
       </c>
       <c r="I232" s="172">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="J232" s="172">
-        <v>168</v>
+        <v>103</v>
       </c>
       <c r="K232" s="172">
-        <v>103</v>
+        <v>146</v>
       </c>
       <c r="L232" s="172">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="M232" s="168">
         <v>0</v>
@@ -68986,8 +68986,8 @@
       <c r="N232" s="169">
         <v>0</v>
       </c>
-      <c r="O232" s="169">
-        <v>0</v>
+      <c r="O232" s="177">
+        <v>2</v>
       </c>
       <c r="P232" s="177">
         <v>0</v>
@@ -68996,7 +68996,7 @@
         <v>0</v>
       </c>
       <c r="R232" s="168">
-        <v>100</v>
+        <v>90.91</v>
       </c>
       <c r="S232" s="169">
         <v>46</v>
@@ -69005,31 +69005,31 @@
         <v>3</v>
       </c>
       <c r="U232" s="169">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="V232" s="169">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W232" s="169">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="X232" s="169">
         <v>2</v>
       </c>
-      <c r="Y232" s="177">
-        <v>39</v>
-      </c>
-      <c r="Z232" s="177">
-        <v>2</v>
+      <c r="Y232" s="169">
+        <v>49</v>
+      </c>
+      <c r="Z232" s="169">
+        <v>3</v>
       </c>
       <c r="AA232" s="169">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="AB232" s="169">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="AC232" s="169">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="AD232" s="173">
         <v>6.9</v>
@@ -69038,15 +69038,15 @@
         <v>6.6</v>
       </c>
       <c r="AF232" s="169" t="s">
-        <v>789</v>
+        <v>792</v>
       </c>
       <c r="AG232" s="170" t="s">
-        <v>790</v>
+        <v>793</v>
       </c>
     </row>
     <row r="233" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="171" t="s">
-        <v>791</v>
+        <v>794</v>
       </c>
       <c r="B233" s="171">
         <v>70</v>
@@ -69055,31 +69055,31 @@
         <v>2</v>
       </c>
       <c r="D233" s="172">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E233" s="172">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F233" s="172">
-        <v>16.5</v>
+        <v>9</v>
       </c>
       <c r="G233" s="172">
-        <v>2.5</v>
+        <v>5.5</v>
       </c>
       <c r="H233" s="215">
-        <v>19</v>
+        <v>14.5</v>
       </c>
       <c r="I233" s="172">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="J233" s="172">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K233" s="172">
-        <v>146</v>
+        <v>109</v>
       </c>
       <c r="L233" s="172">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="M233" s="168">
         <v>0</v>
@@ -69087,67 +69087,67 @@
       <c r="N233" s="169">
         <v>0</v>
       </c>
-      <c r="O233" s="177">
-        <v>2</v>
-      </c>
-      <c r="P233" s="177">
-        <v>0</v>
-      </c>
-      <c r="Q233" s="169">
-        <v>0</v>
+      <c r="O233" s="169">
+        <v>0</v>
+      </c>
+      <c r="P233" s="228">
+        <v>44440</v>
+      </c>
+      <c r="Q233" s="169" t="s">
+        <v>795</v>
       </c>
       <c r="R233" s="168">
-        <v>90.91</v>
-      </c>
-      <c r="S233" s="169">
-        <v>46</v>
-      </c>
-      <c r="T233" s="169">
-        <v>3</v>
-      </c>
-      <c r="U233" s="169">
-        <v>46</v>
+        <v>90.9</v>
+      </c>
+      <c r="S233" s="177">
+        <v>52</v>
+      </c>
+      <c r="T233" s="177">
+        <v>3</v>
+      </c>
+      <c r="U233" s="177">
+        <v>42</v>
       </c>
       <c r="V233" s="169">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W233" s="169">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="X233" s="169">
-        <v>2</v>
-      </c>
-      <c r="Y233" s="169">
-        <v>49</v>
+        <v>3</v>
+      </c>
+      <c r="Y233" s="177">
+        <v>53</v>
       </c>
       <c r="Z233" s="169">
         <v>3</v>
       </c>
-      <c r="AA233" s="169">
-        <v>120</v>
+      <c r="AA233" s="177">
+        <v>114</v>
       </c>
       <c r="AB233" s="169">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="AC233" s="169">
-        <v>123</v>
-      </c>
-      <c r="AD233" s="173">
-        <v>6.9</v>
-      </c>
-      <c r="AE233" s="173">
-        <v>6.6</v>
+        <v>112</v>
+      </c>
+      <c r="AD233" s="168">
+        <v>8</v>
+      </c>
+      <c r="AE233" s="168">
+        <v>7</v>
       </c>
       <c r="AF233" s="169" t="s">
-        <v>792</v>
+        <v>796</v>
       </c>
       <c r="AG233" s="170" t="s">
-        <v>793</v>
+        <v>797</v>
       </c>
     </row>
     <row r="234" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="171" t="s">
-        <v>794</v>
+        <v>798</v>
       </c>
       <c r="B234" s="171">
         <v>70</v>
@@ -69156,31 +69156,31 @@
         <v>2</v>
       </c>
       <c r="D234" s="172">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E234" s="172">
         <v>26</v>
       </c>
       <c r="F234" s="172">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="G234" s="172">
-        <v>5.5</v>
+        <v>2</v>
       </c>
       <c r="H234" s="215">
-        <v>14.5</v>
+        <v>20</v>
       </c>
       <c r="I234" s="172">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="J234" s="172">
-        <v>101</v>
+        <v>143</v>
       </c>
       <c r="K234" s="172">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="L234" s="172">
-        <v>112</v>
+        <v>139</v>
       </c>
       <c r="M234" s="168">
         <v>0</v>
@@ -69191,40 +69191,40 @@
       <c r="O234" s="169">
         <v>0</v>
       </c>
-      <c r="P234" s="228">
-        <v>44440</v>
-      </c>
-      <c r="Q234" s="169" t="s">
-        <v>795</v>
+      <c r="P234" s="227">
+        <v>44563</v>
+      </c>
+      <c r="Q234" s="169">
+        <v>4</v>
       </c>
       <c r="R234" s="168">
-        <v>90.9</v>
+        <v>100</v>
       </c>
       <c r="S234" s="177">
-        <v>52</v>
-      </c>
-      <c r="T234" s="177">
-        <v>3</v>
+        <v>39</v>
+      </c>
+      <c r="T234" s="169">
+        <v>2</v>
       </c>
       <c r="U234" s="177">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="V234" s="169">
         <v>2</v>
       </c>
       <c r="W234" s="169">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="X234" s="169">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Y234" s="177">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="Z234" s="169">
-        <v>3</v>
-      </c>
-      <c r="AA234" s="177">
+        <v>2</v>
+      </c>
+      <c r="AA234" s="169">
         <v>114</v>
       </c>
       <c r="AB234" s="169">
@@ -69234,21 +69234,21 @@
         <v>112</v>
       </c>
       <c r="AD234" s="168">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="AE234" s="168">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="AF234" s="169" t="s">
-        <v>796</v>
+        <v>799</v>
       </c>
       <c r="AG234" s="170" t="s">
-        <v>797</v>
+        <v>800</v>
       </c>
     </row>
     <row r="235" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="171" t="s">
-        <v>798</v>
+        <v>801</v>
       </c>
       <c r="B235" s="171">
         <v>70</v>
@@ -69257,196 +69257,112 @@
         <v>2</v>
       </c>
       <c r="D235" s="172">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E235" s="172">
         <v>26</v>
       </c>
       <c r="F235" s="172">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G235" s="172">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H235" s="215">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="I235" s="172">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="J235" s="172">
-        <v>143</v>
+        <v>94</v>
       </c>
       <c r="K235" s="172">
+        <v>128</v>
+      </c>
+      <c r="L235" s="172">
+        <v>114</v>
+      </c>
+      <c r="M235" s="185">
+        <v>0</v>
+      </c>
+      <c r="N235" s="177">
+        <v>0</v>
+      </c>
+      <c r="O235" s="177">
+        <v>0</v>
+      </c>
+      <c r="P235" s="227">
+        <v>44227</v>
+      </c>
+      <c r="Q235" s="225">
+        <v>45078</v>
+      </c>
+      <c r="R235" s="185">
+        <v>83.33</v>
+      </c>
+      <c r="S235" s="177">
+        <v>48</v>
+      </c>
+      <c r="T235" s="177">
+        <v>3</v>
+      </c>
+      <c r="U235" s="177">
+        <v>42</v>
+      </c>
+      <c r="V235" s="177">
+        <v>2</v>
+      </c>
+      <c r="W235" s="177">
+        <v>52</v>
+      </c>
+      <c r="X235" s="177">
+        <v>3</v>
+      </c>
+      <c r="Y235" s="177">
+        <v>45</v>
+      </c>
+      <c r="Z235" s="177">
+        <v>3</v>
+      </c>
+      <c r="AA235" s="177">
+        <v>108</v>
+      </c>
+      <c r="AB235" s="177">
+        <v>112</v>
+      </c>
+      <c r="AC235" s="177">
         <v>111</v>
       </c>
-      <c r="L235" s="172">
-        <v>139</v>
-      </c>
-      <c r="M235" s="168">
-        <v>0</v>
-      </c>
-      <c r="N235" s="169">
-        <v>0</v>
-      </c>
-      <c r="O235" s="169">
-        <v>0</v>
-      </c>
-      <c r="P235" s="227">
-        <v>44563</v>
-      </c>
-      <c r="Q235" s="169">
-        <v>4</v>
-      </c>
-      <c r="R235" s="168">
-        <v>100</v>
-      </c>
-      <c r="S235" s="177">
-        <v>39</v>
-      </c>
-      <c r="T235" s="169">
-        <v>2</v>
-      </c>
-      <c r="U235" s="177">
-        <v>38</v>
-      </c>
-      <c r="V235" s="169">
-        <v>2</v>
-      </c>
-      <c r="W235" s="169">
-        <v>41</v>
-      </c>
-      <c r="X235" s="169">
-        <v>2</v>
-      </c>
-      <c r="Y235" s="177">
-        <v>38</v>
-      </c>
-      <c r="Z235" s="169">
-        <v>2</v>
-      </c>
-      <c r="AA235" s="169">
-        <v>114</v>
-      </c>
-      <c r="AB235" s="169">
-        <v>107</v>
-      </c>
-      <c r="AC235" s="169">
-        <v>112</v>
-      </c>
-      <c r="AD235" s="168">
-        <v>4</v>
-      </c>
-      <c r="AE235" s="168">
-        <v>4</v>
-      </c>
-      <c r="AF235" s="169" t="s">
-        <v>799</v>
-      </c>
-      <c r="AG235" s="170" t="s">
-        <v>800</v>
+      <c r="AD235" s="185">
+        <v>7</v>
+      </c>
+      <c r="AE235" s="185">
+        <v>7</v>
+      </c>
+      <c r="AF235" s="177" t="s">
+        <v>802</v>
+      </c>
+      <c r="AG235" s="170">
+        <v>5530185775</v>
       </c>
     </row>
     <row r="236" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A236" s="171" t="s">
-        <v>801</v>
-      </c>
-      <c r="B236" s="171">
-        <v>70</v>
-      </c>
-      <c r="C236" s="171">
-        <v>2</v>
-      </c>
-      <c r="D236" s="172">
-        <v>73</v>
-      </c>
-      <c r="E236" s="172">
-        <v>26</v>
-      </c>
-      <c r="F236" s="172">
-        <v>12</v>
-      </c>
-      <c r="G236" s="172">
-        <v>0</v>
-      </c>
-      <c r="H236" s="215">
-        <v>12</v>
-      </c>
-      <c r="I236" s="172">
-        <v>109</v>
-      </c>
-      <c r="J236" s="172">
-        <v>94</v>
-      </c>
-      <c r="K236" s="172">
-        <v>128</v>
-      </c>
-      <c r="L236" s="172">
-        <v>114</v>
-      </c>
-      <c r="M236" s="185">
-        <v>0</v>
-      </c>
-      <c r="N236" s="177">
-        <v>0</v>
-      </c>
-      <c r="O236" s="177">
-        <v>0</v>
-      </c>
-      <c r="P236" s="227">
-        <v>44227</v>
-      </c>
-      <c r="Q236" s="225">
-        <v>45078</v>
-      </c>
-      <c r="R236" s="185">
-        <v>83.33</v>
-      </c>
-      <c r="S236" s="177">
-        <v>48</v>
-      </c>
-      <c r="T236" s="177">
-        <v>3</v>
-      </c>
-      <c r="U236" s="177">
-        <v>42</v>
-      </c>
-      <c r="V236" s="177">
-        <v>2</v>
-      </c>
-      <c r="W236" s="177">
-        <v>52</v>
-      </c>
-      <c r="X236" s="177">
-        <v>3</v>
-      </c>
-      <c r="Y236" s="177">
-        <v>45</v>
-      </c>
-      <c r="Z236" s="177">
-        <v>3</v>
-      </c>
-      <c r="AA236" s="177">
-        <v>108</v>
-      </c>
-      <c r="AB236" s="177">
-        <v>112</v>
-      </c>
-      <c r="AC236" s="177">
-        <v>111</v>
-      </c>
-      <c r="AD236" s="185">
-        <v>7</v>
-      </c>
-      <c r="AE236" s="185">
-        <v>7</v>
-      </c>
-      <c r="AF236" s="177" t="s">
-        <v>802</v>
-      </c>
-      <c r="AG236" s="170">
-        <v>5530185775</v>
-      </c>
+      <c r="N236" s="165"/>
+      <c r="O236" s="165"/>
+      <c r="P236" s="165"/>
+      <c r="Q236" s="165"/>
+      <c r="S236" s="165"/>
+      <c r="T236" s="165"/>
+      <c r="U236" s="165"/>
+      <c r="V236" s="165"/>
+      <c r="W236" s="165"/>
+      <c r="X236" s="165"/>
+      <c r="Y236" s="165"/>
+      <c r="Z236" s="165"/>
+      <c r="AA236" s="165"/>
+      <c r="AB236" s="165"/>
+      <c r="AC236" s="165"/>
     </row>
     <row r="237" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N237" s="165"/>
@@ -69461,24 +69377,8 @@
       <c r="X237" s="165"/>
       <c r="Y237" s="165"/>
       <c r="Z237" s="165"/>
-      <c r="AA237" s="165"/>
-      <c r="AB237" s="165"/>
-      <c r="AC237" s="165"/>
-    </row>
-    <row r="238" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N238" s="165"/>
-      <c r="O238" s="165"/>
-      <c r="P238" s="165"/>
-      <c r="Q238" s="165"/>
-      <c r="S238" s="165"/>
-      <c r="T238" s="165"/>
-      <c r="U238" s="165"/>
-      <c r="V238" s="165"/>
-      <c r="W238" s="165"/>
-      <c r="X238" s="165"/>
-      <c r="Y238" s="165"/>
-      <c r="Z238" s="165"/>
-    </row>
+    </row>
+    <row r="238" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="239" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="240" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="241" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -70200,7 +70100,6 @@
     <row r="957" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="958" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="959" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="960" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>